<commit_message>
added testprocedure and updated Anforderungen
</commit_message>
<xml_diff>
--- a/Anforderungen/Anforderungen.xlsx
+++ b/Anforderungen/Anforderungen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\Mikrocomputertechnik\CO2Messer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\DHBW\Mikrocomputertechnik\CO2Messer\MC_Projekt\Anforderungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA2F539-0649-48CA-84EA-300566759CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036CE1BF-06B4-4C80-909C-4851426D3D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2504784F-D387-4BEC-B9D6-55A8DFAB6B98}"/>
   </bookViews>
@@ -105,13 +105,13 @@
 Luftgüte (Ausgabe LCD)</t>
   </si>
   <si>
-    <t>Benutzer kann Messprofile auswählen (Messprofil: Abtastrate, Grenzwerte)</t>
-  </si>
-  <si>
     <t>Externe Abfrage über USB-Schnittstelle</t>
   </si>
   <si>
     <t>Speichern im CSV-Format</t>
+  </si>
+  <si>
+    <t>Benutzer kann zwischen drei Messprofilen auswählen (Messprofil: Abtastrate)</t>
   </si>
 </sst>
 </file>
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -221,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -270,6 +276,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -589,7 +601,7 @@
   <dimension ref="C2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +635,7 @@
       <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -647,9 +659,9 @@
         <v>3</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -675,7 +687,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>10</v>
@@ -689,7 +701,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
schaltung und anforderungen aktuallisiert und verbessert
</commit_message>
<xml_diff>
--- a/Anforderungen/Anforderungen.xlsx
+++ b/Anforderungen/Anforderungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49157\Documents\DHBW\Mikrocomputertechnik\CO2Messer\MC_Projekt\Anforderungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940C4F00-B56D-4B62-8E51-9BBAEEC1256B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC795474-D6FE-45F7-BC38-60E8B61E5BCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{2504784F-D387-4BEC-B9D6-55A8DFAB6B98}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Nummer</t>
   </si>
@@ -108,6 +108,10 @@
   <si>
     <t>Echtzeitmessung der
 Luftgüte</t>
+  </si>
+  <si>
+    <t>Bei guter Luftgüte:
+Fenster schließt sich (LED aus)</t>
   </si>
 </sst>
 </file>
@@ -588,7 +592,7 @@
   <dimension ref="C2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>6</v>

</xml_diff>